<commit_message>
Inclusão de Normalizações e do Script com o CatBoost
</commit_message>
<xml_diff>
--- a/botafogo_previsao_estadio.xlsx
+++ b/botafogo_previsao_estadio.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9399af9f441dfb25/Documentos/Projeto Futebol/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9399af9f441dfb25/Documentos/Projeto Futebol/ia-botafogo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2885" documentId="8_{FF0F605F-F2C5-4D0A-9132-A4D8069F1A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD2992AD-945A-4D0C-AE27-DD1C6AFCE78E}"/>
+  <xr:revisionPtr revIDLastSave="3029" documentId="8_{FF0F605F-F2C5-4D0A-9132-A4D8069F1A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE10D402-AE09-4C33-9F97-11062DD785B9}"/>
   <bookViews>
-    <workbookView xWindow="36225" yWindow="0" windowWidth="21480" windowHeight="15585" xr2:uid="{BDAF93C4-966A-4323-BFDC-13327AEDDB19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BDAF93C4-966A-4323-BFDC-13327AEDDB19}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$AC$185</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$AC$187</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="130">
   <si>
     <t>ano_campeonato</t>
   </si>
@@ -321,9 +321,6 @@
   </si>
   <si>
     <t>semi-final - taça rio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carioca </t>
   </si>
   <si>
     <t>final - taça rio</t>
@@ -826,11 +823,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301F969D-DFCA-4A79-8310-530A765857C0}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AC185"/>
+  <dimension ref="A1:AC187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="A159" sqref="A159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B160" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E171" sqref="E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -1096,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" hidden="1">
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -1221,7 +1218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:29" hidden="1">
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -1268,7 +1265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:29" hidden="1">
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -1313,7 +1310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:29" hidden="1">
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -1440,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" hidden="1">
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -1650,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" hidden="1">
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>2022</v>
       </c>
@@ -1697,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" hidden="1">
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -1824,7 +1821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" hidden="1">
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -2031,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29" hidden="1">
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>2022</v>
       </c>
@@ -2161,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:29" hidden="1">
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>2022</v>
       </c>
@@ -2206,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" hidden="1">
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>2022</v>
       </c>
@@ -2253,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:29" hidden="1">
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>2022</v>
       </c>
@@ -2463,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:29" hidden="1">
+    <row r="26" spans="1:29">
       <c r="A26">
         <v>2022</v>
       </c>
@@ -2590,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:29" hidden="1">
+    <row r="28" spans="1:29">
       <c r="A28">
         <v>2022</v>
       </c>
@@ -2797,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:29" hidden="1">
+    <row r="31" spans="1:29">
       <c r="A31">
         <v>2022</v>
       </c>
@@ -2927,7 +2924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:29" hidden="1">
+    <row r="33" spans="1:29">
       <c r="A33">
         <v>2022</v>
       </c>
@@ -3134,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:29" hidden="1">
+    <row r="36" spans="1:29">
       <c r="A36">
         <v>2022</v>
       </c>
@@ -3261,7 +3258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:29" hidden="1">
+    <row r="38" spans="1:29">
       <c r="A38">
         <v>2022</v>
       </c>
@@ -3308,7 +3305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:29" hidden="1">
+    <row r="39" spans="1:29">
       <c r="A39">
         <v>2022</v>
       </c>
@@ -3435,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:29" hidden="1">
+    <row r="41" spans="1:29">
       <c r="A41">
         <v>2022</v>
       </c>
@@ -3642,7 +3639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:29" hidden="1">
+    <row r="44" spans="1:29">
       <c r="A44">
         <v>2022</v>
       </c>
@@ -3769,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:29" hidden="1">
+    <row r="46" spans="1:29">
       <c r="A46">
         <v>2022</v>
       </c>
@@ -3896,7 +3893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:29" hidden="1">
+    <row r="48" spans="1:29">
       <c r="A48">
         <v>2023</v>
       </c>
@@ -3937,7 +3934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:29" hidden="1">
+    <row r="49" spans="1:29">
       <c r="A49">
         <v>2023</v>
       </c>
@@ -4020,7 +4017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:29" hidden="1">
+    <row r="50" spans="1:29">
       <c r="A50">
         <v>2023</v>
       </c>
@@ -4061,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:29" hidden="1">
+    <row r="51" spans="1:29">
       <c r="A51">
         <v>2023</v>
       </c>
@@ -4144,7 +4141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:29" hidden="1">
+    <row r="52" spans="1:29">
       <c r="A52">
         <v>2023</v>
       </c>
@@ -4184,7 +4181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:29" hidden="1">
+    <row r="53" spans="1:29">
       <c r="A53">
         <v>2023</v>
       </c>
@@ -4264,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:29" hidden="1">
+    <row r="54" spans="1:29">
       <c r="A54">
         <v>2023</v>
       </c>
@@ -4304,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:29" hidden="1">
+    <row r="55" spans="1:29">
       <c r="A55">
         <v>2023</v>
       </c>
@@ -4387,7 +4384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:29" hidden="1">
+    <row r="56" spans="1:29">
       <c r="A56">
         <v>2023</v>
       </c>
@@ -4433,7 +4430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:29" hidden="1">
+    <row r="57" spans="1:29">
       <c r="A57">
         <v>2023</v>
       </c>
@@ -4473,7 +4470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:29" hidden="1">
+    <row r="58" spans="1:29">
       <c r="A58">
         <v>2023</v>
       </c>
@@ -4553,7 +4550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:29" hidden="1">
+    <row r="59" spans="1:29">
       <c r="A59">
         <v>2023</v>
       </c>
@@ -4636,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:29" hidden="1">
+    <row r="60" spans="1:29">
       <c r="A60">
         <v>2023</v>
       </c>
@@ -4682,12 +4679,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:29" hidden="1">
+    <row r="61" spans="1:29">
       <c r="A61">
         <v>2023</v>
       </c>
       <c r="B61" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>93</v>
@@ -4765,7 +4762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:29" hidden="1">
+    <row r="62" spans="1:29">
       <c r="A62">
         <v>2023</v>
       </c>
@@ -4773,7 +4770,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E62" s="1">
         <v>45018</v>
@@ -4811,15 +4808,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:29" hidden="1">
+    <row r="63" spans="1:29">
       <c r="A63">
         <v>2023</v>
       </c>
       <c r="B63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="E63" s="1">
         <v>45022</v>
@@ -4830,7 +4827,7 @@
         <v>1</v>
       </c>
       <c r="S63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T63" t="s">
         <v>35</v>
@@ -4859,7 +4856,7 @@
         <v>29</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D64" t="s">
         <v>31</v>
@@ -4937,7 +4934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:29" hidden="1">
+    <row r="65" spans="1:29">
       <c r="A65">
         <v>2023</v>
       </c>
@@ -4959,7 +4956,7 @@
         <v>38</v>
       </c>
       <c r="S65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T65" t="s">
         <v>35</v>
@@ -5068,10 +5065,10 @@
         <v>2023</v>
       </c>
       <c r="B67" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="D67" t="s">
         <v>31</v>
@@ -5119,10 +5116,10 @@
         <v>35</v>
       </c>
       <c r="T67" t="s">
+        <v>99</v>
+      </c>
+      <c r="U67" t="s">
         <v>100</v>
-      </c>
-      <c r="U67" t="s">
-        <v>101</v>
       </c>
       <c r="X67" t="s">
         <v>47</v>
@@ -5143,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:29" hidden="1">
+    <row r="68" spans="1:29">
       <c r="A68">
         <v>2023</v>
       </c>
@@ -5169,7 +5166,7 @@
         <v>47364</v>
       </c>
       <c r="S68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T68" t="s">
         <v>35</v>
@@ -5249,7 +5246,7 @@
         <v>35</v>
       </c>
       <c r="T69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U69" t="s">
         <v>54</v>
@@ -5276,7 +5273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:29" hidden="1">
+    <row r="70" spans="1:29">
       <c r="A70">
         <v>2023</v>
       </c>
@@ -5325,10 +5322,10 @@
         <v>2023</v>
       </c>
       <c r="B71" t="s">
+        <v>95</v>
+      </c>
+      <c r="C71" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="D71" t="s">
         <v>31</v>
@@ -5376,10 +5373,10 @@
         <v>35</v>
       </c>
       <c r="T71" t="s">
+        <v>102</v>
+      </c>
+      <c r="U71" t="s">
         <v>103</v>
-      </c>
-      <c r="U71" t="s">
-        <v>104</v>
       </c>
       <c r="X71" t="s">
         <v>47</v>
@@ -5563,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:29" hidden="1">
+    <row r="74" spans="1:29">
       <c r="A74">
         <v>2023</v>
       </c>
@@ -5610,7 +5607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:29" hidden="1">
+    <row r="75" spans="1:29">
       <c r="A75">
         <v>2023</v>
       </c>
@@ -5740,15 +5737,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:29" hidden="1">
+    <row r="77" spans="1:29">
       <c r="A77">
         <v>2023</v>
       </c>
       <c r="B77" t="s">
+        <v>95</v>
+      </c>
+      <c r="C77" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="E77" s="1">
         <v>45071</v>
@@ -5759,7 +5756,7 @@
         <v>4</v>
       </c>
       <c r="S77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T77" t="s">
         <v>35</v>
@@ -5943,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:29" hidden="1">
+    <row r="80" spans="1:29">
       <c r="A80">
         <v>2023</v>
       </c>
@@ -5993,15 +5990,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:29" hidden="1">
+    <row r="81" spans="1:29">
       <c r="A81">
         <v>2023</v>
       </c>
       <c r="B81" t="s">
+        <v>95</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="E81" s="1">
         <v>45083</v>
@@ -6013,7 +6010,7 @@
         <v>5</v>
       </c>
       <c r="S81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T81" t="s">
         <v>35</v>
@@ -6114,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:29" hidden="1">
+    <row r="83" spans="1:29">
       <c r="A83">
         <v>2023</v>
       </c>
@@ -6161,7 +6158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:29" hidden="1">
+    <row r="84" spans="1:29">
       <c r="A84">
         <v>2023</v>
       </c>
@@ -6213,10 +6210,10 @@
         <v>2023</v>
       </c>
       <c r="B85" t="s">
+        <v>95</v>
+      </c>
+      <c r="C85" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="D85" t="s">
         <v>31</v>
@@ -6252,10 +6249,10 @@
         <v>35</v>
       </c>
       <c r="T85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X85" t="s">
         <v>47</v>
@@ -6341,7 +6338,7 @@
         <v>33</v>
       </c>
       <c r="X86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y86">
         <v>6</v>
@@ -6359,7 +6356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:29" hidden="1">
+    <row r="87" spans="1:29">
       <c r="A87">
         <v>2023</v>
       </c>
@@ -6385,13 +6382,13 @@
         <v>60540</v>
       </c>
       <c r="S87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T87" t="s">
         <v>35</v>
       </c>
       <c r="X87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Z87">
         <v>2</v>
@@ -6406,12 +6403,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:29" hidden="1">
+    <row r="88" spans="1:29">
       <c r="A88">
         <v>2023</v>
       </c>
       <c r="B88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>90</v>
@@ -6429,7 +6426,7 @@
         <v>38</v>
       </c>
       <c r="S88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T88" t="s">
         <v>35</v>
@@ -6438,7 +6435,7 @@
         <v>33</v>
       </c>
       <c r="X88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Z88">
         <v>0</v>
@@ -6515,7 +6512,7 @@
         <v>46</v>
       </c>
       <c r="X89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Y89">
         <v>5</v>
@@ -6538,7 +6535,7 @@
         <v>2023</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>90</v>
@@ -6580,16 +6577,16 @@
         <v>35</v>
       </c>
       <c r="T90" t="s">
+        <v>107</v>
+      </c>
+      <c r="U90" t="s">
         <v>108</v>
-      </c>
-      <c r="U90" t="s">
-        <v>109</v>
       </c>
       <c r="W90" t="s">
         <v>33</v>
       </c>
       <c r="X90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y90">
         <v>6</v>
@@ -6607,7 +6604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:29" hidden="1">
+    <row r="91" spans="1:29">
       <c r="A91">
         <v>2023</v>
       </c>
@@ -6639,7 +6636,7 @@
         <v>35</v>
       </c>
       <c r="X91" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z91">
         <v>13</v>
@@ -6716,7 +6713,7 @@
         <v>75</v>
       </c>
       <c r="X92" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y92">
         <v>6</v>
@@ -6739,7 +6736,7 @@
         <v>2023</v>
       </c>
       <c r="B93" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>68</v>
@@ -6781,16 +6778,16 @@
         <v>35</v>
       </c>
       <c r="T93" t="s">
+        <v>110</v>
+      </c>
+      <c r="U93" t="s">
         <v>111</v>
-      </c>
-      <c r="U93" t="s">
-        <v>112</v>
       </c>
       <c r="W93" t="s">
         <v>33</v>
       </c>
       <c r="X93" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y93">
         <v>5</v>
@@ -6808,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:29" hidden="1">
+    <row r="94" spans="1:29">
       <c r="A94">
         <v>2023</v>
       </c>
@@ -6834,13 +6831,13 @@
         <v>61927</v>
       </c>
       <c r="S94" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T94" t="s">
         <v>35</v>
       </c>
       <c r="X94" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z94">
         <v>10</v>
@@ -6855,12 +6852,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:29" hidden="1">
+    <row r="95" spans="1:29">
       <c r="A95">
         <v>2023</v>
       </c>
       <c r="B95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>68</v>
@@ -6881,7 +6878,7 @@
         <v>33</v>
       </c>
       <c r="S95" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T95" t="s">
         <v>35</v>
@@ -6890,7 +6887,7 @@
         <v>33</v>
       </c>
       <c r="X95" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z95">
         <v>2</v>
@@ -6967,7 +6964,7 @@
         <v>54</v>
       </c>
       <c r="X96" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y96">
         <v>6</v>
@@ -6985,7 +6982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:29" hidden="1">
+    <row r="97" spans="1:29">
       <c r="A97">
         <v>2023</v>
       </c>
@@ -7017,7 +7014,7 @@
         <v>35</v>
       </c>
       <c r="X97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z97">
         <v>9</v>
@@ -7037,10 +7034,10 @@
         <v>2023</v>
       </c>
       <c r="B98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D98" t="s">
         <v>31</v>
@@ -7079,16 +7076,16 @@
         <v>35</v>
       </c>
       <c r="T98" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U98" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W98" t="s">
         <v>33</v>
       </c>
       <c r="X98" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y98">
         <v>7</v>
@@ -7162,13 +7159,13 @@
         <v>35</v>
       </c>
       <c r="T99" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U99" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y99">
         <v>7</v>
@@ -7186,15 +7183,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:29" hidden="1">
+    <row r="100" spans="1:29">
       <c r="A100">
         <v>2023</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C100" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E100" s="1">
         <v>45168</v>
@@ -7208,7 +7205,7 @@
         <v>42</v>
       </c>
       <c r="S100" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T100" t="s">
         <v>35</v>
@@ -7217,7 +7214,7 @@
         <v>33</v>
       </c>
       <c r="X100" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z100">
         <v>1</v>
@@ -7297,7 +7294,7 @@
         <v>33</v>
       </c>
       <c r="X101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y101">
         <v>2</v>
@@ -7315,7 +7312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:29" hidden="1">
+    <row r="102" spans="1:29">
       <c r="A102">
         <v>2023</v>
       </c>
@@ -7347,7 +7344,7 @@
         <v>35</v>
       </c>
       <c r="X102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z102">
         <v>9</v>
@@ -7362,7 +7359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:29" hidden="1">
+    <row r="103" spans="1:29">
       <c r="A103">
         <v>2023</v>
       </c>
@@ -7394,7 +7391,7 @@
         <v>35</v>
       </c>
       <c r="X103" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Z103">
         <v>12</v>
@@ -7471,7 +7468,7 @@
         <v>62</v>
       </c>
       <c r="X104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y104">
         <v>3</v>
@@ -7489,7 +7486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:29" hidden="1">
+    <row r="105" spans="1:29">
       <c r="A105">
         <v>2023</v>
       </c>
@@ -7536,7 +7533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:29" hidden="1">
+    <row r="106" spans="1:29">
       <c r="A106">
         <v>2023</v>
       </c>
@@ -7823,7 +7820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:29" hidden="1">
+    <row r="110" spans="1:29">
       <c r="A110">
         <v>2023</v>
       </c>
@@ -7862,7 +7859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:29" hidden="1">
+    <row r="111" spans="1:29">
       <c r="A111">
         <v>2023</v>
       </c>
@@ -7873,7 +7870,7 @@
         <v>44</v>
       </c>
       <c r="D111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E111" s="1">
         <v>45239</v>
@@ -7918,7 +7915,7 @@
         <v>35</v>
       </c>
       <c r="T111" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U111" t="s">
         <v>54</v>
@@ -7942,7 +7939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:29" hidden="1">
+    <row r="112" spans="1:29">
       <c r="A112">
         <v>2023</v>
       </c>
@@ -7981,7 +7978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:29" hidden="1">
+    <row r="113" spans="1:29">
       <c r="A113">
         <v>2023</v>
       </c>
@@ -8005,7 +8002,7 @@
         <v>35</v>
       </c>
       <c r="X113" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z113">
         <v>9</v>
@@ -8082,7 +8079,7 @@
         <v>46</v>
       </c>
       <c r="X114" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y114">
         <v>4</v>
@@ -8100,7 +8097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:29" hidden="1">
+    <row r="115" spans="1:29">
       <c r="A115">
         <v>2023</v>
       </c>
@@ -8124,7 +8121,7 @@
         <v>35</v>
       </c>
       <c r="X115" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z115">
         <v>3</v>
@@ -8195,13 +8192,13 @@
         <v>35</v>
       </c>
       <c r="T116" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U116" t="s">
         <v>71</v>
       </c>
       <c r="X116" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y116">
         <v>5</v>
@@ -8219,7 +8216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:29" hidden="1">
+    <row r="117" spans="1:29">
       <c r="A117">
         <v>2023</v>
       </c>
@@ -8243,7 +8240,7 @@
         <v>35</v>
       </c>
       <c r="X117" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z117">
         <v>9</v>
@@ -8320,7 +8317,7 @@
         <v>40</v>
       </c>
       <c r="X118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y118">
         <v>3</v>
@@ -8403,7 +8400,7 @@
         <v>40</v>
       </c>
       <c r="X119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y119">
         <v>4</v>
@@ -8421,7 +8418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:29" hidden="1">
+    <row r="120" spans="1:29">
       <c r="A120">
         <v>2024</v>
       </c>
@@ -8446,7 +8443,7 @@
         <v>35</v>
       </c>
       <c r="X120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z120">
         <v>1</v>
@@ -8520,13 +8517,13 @@
         <v>35</v>
       </c>
       <c r="T121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U121" t="s">
         <v>40</v>
       </c>
       <c r="X121" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y121">
         <v>3</v>
@@ -8606,7 +8603,7 @@
         <v>40</v>
       </c>
       <c r="X122" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y122">
         <v>3</v>
@@ -8624,7 +8621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:29" hidden="1">
+    <row r="123" spans="1:29">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -8635,7 +8632,7 @@
         <v>44</v>
       </c>
       <c r="D123" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E123" s="1">
         <v>45325</v>
@@ -8686,7 +8683,7 @@
         <v>40</v>
       </c>
       <c r="X123" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y123">
         <v>6</v>
@@ -8704,7 +8701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:29" hidden="1">
+    <row r="124" spans="1:29">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -8729,7 +8726,7 @@
         <v>35</v>
       </c>
       <c r="X124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z124">
         <v>2</v>
@@ -8744,7 +8741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:29" hidden="1">
+    <row r="125" spans="1:29">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -8769,7 +8766,7 @@
         <v>35</v>
       </c>
       <c r="X125" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z125">
         <v>9</v>
@@ -8852,7 +8849,7 @@
         <v>33</v>
       </c>
       <c r="X126" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y126">
         <v>9</v>
@@ -8870,12 +8867,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:29" hidden="1">
+    <row r="127" spans="1:29">
       <c r="A127">
         <v>2024</v>
       </c>
       <c r="B127" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>90</v>
@@ -8892,7 +8889,7 @@
         <v>38</v>
       </c>
       <c r="S127" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T127" t="s">
         <v>35</v>
@@ -8901,7 +8898,7 @@
         <v>33</v>
       </c>
       <c r="X127" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Z127">
         <v>0</v>
@@ -8916,7 +8913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:29" hidden="1">
+    <row r="128" spans="1:29">
       <c r="A128">
         <v>2024</v>
       </c>
@@ -8944,7 +8941,7 @@
         <v>35</v>
       </c>
       <c r="X128" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z128">
         <v>12</v>
@@ -8964,7 +8961,7 @@
         <v>2024</v>
       </c>
       <c r="B129" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>90</v>
@@ -9003,16 +9000,16 @@
         <v>35</v>
       </c>
       <c r="T129" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W129" t="s">
         <v>33</v>
       </c>
       <c r="X129" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y129">
         <v>7</v>
@@ -9030,7 +9027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1">
+    <row r="130" spans="1:29">
       <c r="A130">
         <v>2024</v>
       </c>
@@ -9058,7 +9055,7 @@
         <v>35</v>
       </c>
       <c r="X130" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z130">
         <v>2</v>
@@ -9078,7 +9075,7 @@
         <v>2024</v>
       </c>
       <c r="B131" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C131" t="s">
         <v>50</v>
@@ -9126,7 +9123,7 @@
         <v>33</v>
       </c>
       <c r="X131" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y131">
         <v>7</v>
@@ -9144,7 +9141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1">
+    <row r="132" spans="1:29">
       <c r="A132">
         <v>2024</v>
       </c>
@@ -9169,7 +9166,7 @@
         <v>33</v>
       </c>
       <c r="S132" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T132" t="s">
         <v>35</v>
@@ -9178,7 +9175,7 @@
         <v>33</v>
       </c>
       <c r="X132" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z132">
         <v>0</v>
@@ -9193,12 +9190,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1">
+    <row r="133" spans="1:29">
       <c r="A133">
         <v>2024</v>
       </c>
       <c r="B133" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C133" t="s">
         <v>50</v>
@@ -9224,7 +9221,7 @@
         <v>33</v>
       </c>
       <c r="X133" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z133">
         <v>2</v>
@@ -9298,7 +9295,7 @@
         <v>35</v>
       </c>
       <c r="T134" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="U134" t="s">
         <v>40</v>
@@ -9307,7 +9304,7 @@
         <v>33</v>
       </c>
       <c r="X134" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y134">
         <v>9</v>
@@ -9325,7 +9322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1">
+    <row r="135" spans="1:29">
       <c r="A135">
         <v>2024</v>
       </c>
@@ -9333,7 +9330,7 @@
         <v>29</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E135" s="1">
         <v>45378</v>
@@ -9362,7 +9359,7 @@
         <v>33</v>
       </c>
       <c r="X135" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z135">
         <v>0</v>
@@ -9385,7 +9382,7 @@
         <v>29</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D136" t="s">
         <v>31</v>
@@ -9445,7 +9442,7 @@
         <v>33</v>
       </c>
       <c r="X136" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y136">
         <v>3</v>
@@ -9468,10 +9465,10 @@
         <v>2024</v>
       </c>
       <c r="B137" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D137" t="s">
         <v>31</v>
@@ -9507,13 +9504,13 @@
         <v>35</v>
       </c>
       <c r="T137" t="s">
+        <v>124</v>
+      </c>
+      <c r="U137" t="s">
         <v>125</v>
       </c>
-      <c r="U137" t="s">
-        <v>126</v>
-      </c>
       <c r="X137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Y137">
         <v>4</v>
@@ -9531,15 +9528,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1">
+    <row r="138" spans="1:29">
       <c r="A138">
         <v>2024</v>
       </c>
       <c r="B138" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E138" s="1">
         <v>45393</v>
@@ -9553,13 +9550,13 @@
         <v>2</v>
       </c>
       <c r="S138" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T138" t="s">
         <v>35</v>
       </c>
       <c r="X138" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z138">
         <v>3</v>
@@ -9574,7 +9571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1">
+    <row r="139" spans="1:29">
       <c r="A139">
         <v>2024</v>
       </c>
@@ -9593,13 +9590,13 @@
         <v>1</v>
       </c>
       <c r="S139" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T139" t="s">
         <v>35</v>
       </c>
       <c r="X139" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z139">
         <v>0</v>
@@ -9676,7 +9673,7 @@
         <v>62</v>
       </c>
       <c r="X140" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y140">
         <v>6</v>
@@ -9759,7 +9756,7 @@
         <v>54</v>
       </c>
       <c r="X141" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y141">
         <v>4</v>
@@ -9782,10 +9779,10 @@
         <v>2024</v>
       </c>
       <c r="B142" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D142" t="s">
         <v>31</v>
@@ -9821,13 +9818,13 @@
         <v>35</v>
       </c>
       <c r="T142" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U142" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X142" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y142">
         <v>5</v>
@@ -9845,7 +9842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:29" hidden="1">
+    <row r="143" spans="1:29">
       <c r="A143">
         <v>2024</v>
       </c>
@@ -9882,7 +9879,7 @@
         <v>33</v>
       </c>
       <c r="X143" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z143">
         <v>2</v>
@@ -9953,16 +9950,16 @@
         <v>35</v>
       </c>
       <c r="T144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U144" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W144" t="s">
         <v>33</v>
       </c>
       <c r="X144" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y144">
         <v>7</v>
@@ -10039,13 +10036,13 @@
         <v>35</v>
       </c>
       <c r="T145" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U145" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X145" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y145">
         <v>8</v>
@@ -10068,10 +10065,10 @@
         <v>2024</v>
       </c>
       <c r="B146" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D146" t="s">
         <v>31</v>
@@ -10107,13 +10104,13 @@
         <v>35</v>
       </c>
       <c r="T146" t="s">
+        <v>102</v>
+      </c>
+      <c r="U146" t="s">
         <v>103</v>
       </c>
-      <c r="U146" t="s">
-        <v>104</v>
-      </c>
       <c r="X146" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y146">
         <v>8</v>
@@ -10131,7 +10128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:29" hidden="1">
+    <row r="147" spans="1:29">
       <c r="A147">
         <v>2024</v>
       </c>
@@ -10159,7 +10156,7 @@
         <v>35</v>
       </c>
       <c r="X147" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z147">
         <v>12</v>
@@ -10174,15 +10171,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:29" hidden="1">
+    <row r="148" spans="1:29">
       <c r="A148">
         <v>2024</v>
       </c>
       <c r="B148" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E148" s="1">
         <v>45428</v>
@@ -10196,13 +10193,13 @@
         <v>5</v>
       </c>
       <c r="S148" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T148" t="s">
         <v>35</v>
       </c>
       <c r="X148" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z148">
         <v>3</v>
@@ -10217,7 +10214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:29" hidden="1">
+    <row r="149" spans="1:29">
       <c r="A149">
         <v>2024</v>
       </c>
@@ -10239,7 +10236,7 @@
         <v>2</v>
       </c>
       <c r="S149" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T149" t="s">
         <v>35</v>
@@ -10248,7 +10245,7 @@
         <v>33</v>
       </c>
       <c r="X149" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z149">
         <v>2</v>
@@ -10263,15 +10260,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:29" hidden="1">
+    <row r="150" spans="1:29">
       <c r="A150">
         <v>2024</v>
       </c>
       <c r="B150" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E150" s="1">
         <v>45440</v>
@@ -10285,13 +10282,13 @@
         <v>6</v>
       </c>
       <c r="S150" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T150" t="s">
         <v>35</v>
       </c>
       <c r="X150" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z150">
         <v>1</v>
@@ -10306,7 +10303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:29" hidden="1">
+    <row r="151" spans="1:29">
       <c r="A151">
         <v>2024</v>
       </c>
@@ -10334,7 +10331,7 @@
         <v>35</v>
       </c>
       <c r="X151" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z151">
         <v>16</v>
@@ -10414,7 +10411,7 @@
         <v>33</v>
       </c>
       <c r="X152" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y152">
         <v>8</v>
@@ -10432,7 +10429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:29" hidden="1">
+    <row r="153" spans="1:29">
       <c r="A153">
         <v>2024</v>
       </c>
@@ -10454,13 +10451,13 @@
         <v>9</v>
       </c>
       <c r="S153" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T153" t="s">
         <v>35</v>
       </c>
       <c r="X153" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z153">
         <v>3</v>
@@ -10537,7 +10534,7 @@
         <v>75</v>
       </c>
       <c r="X154" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y154">
         <v>5</v>
@@ -10555,7 +10552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:29" hidden="1">
+    <row r="155" spans="1:29">
       <c r="A155">
         <v>2024</v>
       </c>
@@ -10577,13 +10574,13 @@
         <v>11</v>
       </c>
       <c r="S155" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T155" t="s">
         <v>35</v>
       </c>
       <c r="X155" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z155">
         <v>2</v>
@@ -10660,7 +10657,7 @@
         <v>46</v>
       </c>
       <c r="X156" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y156">
         <v>8</v>
@@ -10678,7 +10675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:29" hidden="1">
+    <row r="157" spans="1:29">
       <c r="A157">
         <v>2024</v>
       </c>
@@ -10706,14 +10703,14 @@
         <v>35</v>
       </c>
       <c r="X157" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z157">
+        <v>15</v>
+      </c>
+      <c r="AA157">
         <v>3</v>
       </c>
-      <c r="AA157">
-        <v>15</v>
-      </c>
       <c r="AB157">
         <v>1</v>
       </c>
@@ -10721,7 +10718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:29" hidden="1">
+    <row r="158" spans="1:29">
       <c r="A158">
         <v>2024</v>
       </c>
@@ -10749,7 +10746,7 @@
         <v>35</v>
       </c>
       <c r="X158" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z158">
         <v>14</v>
@@ -10795,9 +10792,27 @@
       <c r="J159" t="s">
         <v>44</v>
       </c>
+      <c r="K159">
+        <v>21582</v>
+      </c>
       <c r="L159">
         <v>46931</v>
       </c>
+      <c r="M159">
+        <v>910175</v>
+      </c>
+      <c r="N159">
+        <v>855916.94</v>
+      </c>
+      <c r="O159">
+        <v>3681.62</v>
+      </c>
+      <c r="P159">
+        <v>54258.06</v>
+      </c>
+      <c r="Q159">
+        <v>54258.06</v>
+      </c>
       <c r="S159" t="s">
         <v>35</v>
       </c>
@@ -10808,7 +10823,7 @@
         <v>71</v>
       </c>
       <c r="X159" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Y159">
         <v>5</v>
@@ -10819,8 +10834,14 @@
       <c r="AA159">
         <v>11</v>
       </c>
-    </row>
-    <row r="160" spans="1:29" hidden="1">
+      <c r="AB159">
+        <v>3</v>
+      </c>
+      <c r="AC159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:29">
       <c r="A160">
         <v>2024</v>
       </c>
@@ -10842,13 +10863,28 @@
         <v>16</v>
       </c>
       <c r="S160" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T160" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="161" spans="1:23">
+      <c r="X160" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z160">
+        <v>15</v>
+      </c>
+      <c r="AA160">
+        <v>2</v>
+      </c>
+      <c r="AB160">
+        <v>0</v>
+      </c>
+      <c r="AC160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:29">
       <c r="A161">
         <v>2024</v>
       </c>
@@ -10867,6 +10903,9 @@
       <c r="F161" s="3">
         <v>0.89583333333333337</v>
       </c>
+      <c r="G161">
+        <v>20</v>
+      </c>
       <c r="H161">
         <v>2</v>
       </c>
@@ -10876,9 +10915,27 @@
       <c r="J161" t="s">
         <v>44</v>
       </c>
+      <c r="K161">
+        <v>39570</v>
+      </c>
       <c r="L161">
         <v>46931</v>
       </c>
+      <c r="M161">
+        <v>2545730</v>
+      </c>
+      <c r="N161">
+        <v>1643530.86</v>
+      </c>
+      <c r="O161">
+        <v>2401.83</v>
+      </c>
+      <c r="P161">
+        <v>902199.14</v>
+      </c>
+      <c r="Q161">
+        <v>902199.14</v>
+      </c>
       <c r="S161" t="s">
         <v>35</v>
       </c>
@@ -10888,8 +10945,26 @@
       <c r="U161" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="162" spans="1:23">
+      <c r="X161" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y161">
+        <v>8</v>
+      </c>
+      <c r="Z161">
+        <v>1</v>
+      </c>
+      <c r="AA161">
+        <v>2</v>
+      </c>
+      <c r="AB161">
+        <v>1</v>
+      </c>
+      <c r="AC161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:29">
       <c r="A162">
         <v>2024</v>
       </c>
@@ -10908,6 +10983,9 @@
       <c r="F162" s="3">
         <v>0.77083333333333337</v>
       </c>
+      <c r="G162">
+        <v>21</v>
+      </c>
       <c r="H162">
         <v>3</v>
       </c>
@@ -10917,9 +10995,27 @@
       <c r="J162" t="s">
         <v>44</v>
       </c>
+      <c r="K162">
+        <v>31344</v>
+      </c>
       <c r="L162">
         <v>46931</v>
       </c>
+      <c r="M162">
+        <v>1773090</v>
+      </c>
+      <c r="N162">
+        <v>1208857.95</v>
+      </c>
+      <c r="O162">
+        <v>3829.63</v>
+      </c>
+      <c r="P162">
+        <v>564232.05000000005</v>
+      </c>
+      <c r="Q162">
+        <v>564232.05000000005</v>
+      </c>
       <c r="S162" t="s">
         <v>35</v>
       </c>
@@ -10929,8 +11025,26 @@
       <c r="U162" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="163" spans="1:23" hidden="1">
+      <c r="X162" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y162">
+        <v>8</v>
+      </c>
+      <c r="Z162">
+        <v>1</v>
+      </c>
+      <c r="AA162">
+        <v>13</v>
+      </c>
+      <c r="AB162">
+        <v>1</v>
+      </c>
+      <c r="AC162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:29">
       <c r="A163">
         <v>2024</v>
       </c>
@@ -10957,8 +11071,23 @@
       <c r="T163" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="164" spans="1:23">
+      <c r="X163" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z163">
+        <v>5</v>
+      </c>
+      <c r="AA163">
+        <v>1</v>
+      </c>
+      <c r="AB163">
+        <v>2</v>
+      </c>
+      <c r="AC163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:29">
       <c r="A164">
         <v>2024</v>
       </c>
@@ -10974,6 +11103,12 @@
       <c r="E164" s="1">
         <v>45500</v>
       </c>
+      <c r="F164" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="G164">
+        <v>22</v>
+      </c>
       <c r="H164">
         <v>4</v>
       </c>
@@ -10983,45 +11118,130 @@
       <c r="J164" t="s">
         <v>44</v>
       </c>
+      <c r="K164">
+        <v>19349</v>
+      </c>
       <c r="L164">
         <v>46931</v>
       </c>
+      <c r="M164">
+        <v>1085780</v>
+      </c>
+      <c r="N164">
+        <v>1018037.97</v>
+      </c>
+      <c r="O164">
+        <v>3776.07</v>
+      </c>
+      <c r="P164">
+        <v>67742.03</v>
+      </c>
+      <c r="Q164">
+        <v>67742.03</v>
+      </c>
+      <c r="R164" t="s">
+        <v>33</v>
+      </c>
       <c r="S164" t="s">
         <v>35</v>
       </c>
       <c r="T164" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U164" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="165" spans="1:23" hidden="1">
+      <c r="X164" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y164">
+        <v>10</v>
+      </c>
+      <c r="Z164">
+        <v>1</v>
+      </c>
+      <c r="AA164">
+        <v>5</v>
+      </c>
+      <c r="AB164">
+        <v>0</v>
+      </c>
+      <c r="AC164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:29">
       <c r="A165">
         <v>2024</v>
       </c>
       <c r="B165" t="s">
-        <v>43</v>
-      </c>
-      <c r="C165" t="s">
-        <v>44</v>
+        <v>49</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D165" t="s">
+        <v>31</v>
       </c>
       <c r="E165" s="1">
-        <v>45507</v>
-      </c>
-      <c r="G165" s="3"/>
-      <c r="H165" s="3"/>
+        <v>45503</v>
+      </c>
+      <c r="F165" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="G165">
+        <v>20</v>
+      </c>
+      <c r="H165">
+        <v>5</v>
+      </c>
       <c r="I165">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="J165" t="s">
+        <v>38</v>
+      </c>
+      <c r="K165">
+        <v>19121</v>
+      </c>
+      <c r="L165">
+        <v>46931</v>
+      </c>
+      <c r="M165">
+        <v>1100400</v>
       </c>
       <c r="S165" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="T165" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="166" spans="1:23" hidden="1">
+        <v>101</v>
+      </c>
+      <c r="U165" t="s">
+        <v>115</v>
+      </c>
+      <c r="W165" t="s">
+        <v>33</v>
+      </c>
+      <c r="X165" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y165">
+        <v>10</v>
+      </c>
+      <c r="Z165">
+        <v>0</v>
+      </c>
+      <c r="AA165">
+        <v>0</v>
+      </c>
+      <c r="AB165">
+        <v>1</v>
+      </c>
+      <c r="AC165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:29">
       <c r="A166">
         <v>2024</v>
       </c>
@@ -11032,62 +11252,82 @@
         <v>44</v>
       </c>
       <c r="E166" s="1">
-        <v>45514</v>
+        <v>45507</v>
+      </c>
+      <c r="F166" s="3">
+        <v>0.83333333333333337</v>
       </c>
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
       <c r="I166">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S166" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T166" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="167" spans="1:23">
+      <c r="Z166">
+        <v>20</v>
+      </c>
+      <c r="AA166">
+        <v>2</v>
+      </c>
+      <c r="AB166">
+        <v>1</v>
+      </c>
+      <c r="AC166">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:29">
       <c r="A167">
         <v>2024</v>
       </c>
       <c r="B167" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="C167" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D167" t="s">
-        <v>31</v>
-      </c>
       <c r="E167" s="1">
-        <v>45518</v>
-      </c>
-      <c r="H167">
-        <v>1</v>
-      </c>
+        <v>45511</v>
+      </c>
+      <c r="F167" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="G167" s="3"/>
+      <c r="H167" s="3"/>
       <c r="I167">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J167" t="s">
-        <v>38</v>
-      </c>
-      <c r="L167">
-        <v>46931</v>
+        <v>42</v>
       </c>
       <c r="S167" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="T167" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="U167" t="s">
-        <v>46</v>
-      </c>
-      <c r="W167" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="168" spans="1:23">
+        <v>115</v>
+      </c>
+      <c r="Z167">
+        <v>1</v>
+      </c>
+      <c r="AA167">
+        <v>2</v>
+      </c>
+      <c r="AB167">
+        <v>1</v>
+      </c>
+      <c r="AC167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:29">
       <c r="A168">
         <v>2024</v>
       </c>
@@ -11097,66 +11337,108 @@
       <c r="C168" t="s">
         <v>44</v>
       </c>
-      <c r="D168" t="s">
-        <v>31</v>
-      </c>
       <c r="E168" s="1">
-        <v>45521</v>
-      </c>
-      <c r="H168">
-        <v>2</v>
-      </c>
+        <v>45514</v>
+      </c>
+      <c r="F168" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G168" s="3"/>
+      <c r="H168" s="3"/>
       <c r="I168">
-        <v>23</v>
-      </c>
-      <c r="J168" t="s">
-        <v>44</v>
-      </c>
-      <c r="L168">
-        <v>46931</v>
+        <v>22</v>
       </c>
       <c r="S168" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="T168" t="s">
-        <v>55</v>
-      </c>
-      <c r="U168" t="s">
-        <v>40</v>
-      </c>
-      <c r="V168" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="169" spans="1:23" hidden="1">
+        <v>35</v>
+      </c>
+      <c r="Z168">
+        <v>13</v>
+      </c>
+      <c r="AA168">
+        <v>1</v>
+      </c>
+      <c r="AB168">
+        <v>3</v>
+      </c>
+      <c r="AC168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:29">
       <c r="A169">
         <v>2024</v>
       </c>
       <c r="B169" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="D169" t="s">
+        <v>31</v>
+      </c>
       <c r="E169" s="1">
-        <v>45525</v>
-      </c>
-      <c r="G169" s="3"/>
-      <c r="H169" s="3"/>
+        <v>45518</v>
+      </c>
+      <c r="F169" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="G169">
+        <v>20</v>
+      </c>
+      <c r="H169">
+        <v>1</v>
+      </c>
       <c r="I169">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J169" t="s">
+        <v>38</v>
+      </c>
+      <c r="K169">
+        <v>38848</v>
+      </c>
+      <c r="L169">
+        <v>46931</v>
+      </c>
+      <c r="M169">
+        <v>1775401.25</v>
       </c>
       <c r="S169" t="s">
+        <v>35</v>
+      </c>
+      <c r="T169" t="s">
         <v>63</v>
       </c>
-      <c r="T169" t="s">
-        <v>35</v>
+      <c r="U169" t="s">
+        <v>46</v>
       </c>
       <c r="W169" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="170" spans="1:23" hidden="1">
+      <c r="X169" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y169">
+        <v>6</v>
+      </c>
+      <c r="Z169">
+        <v>0</v>
+      </c>
+      <c r="AA169">
+        <v>0</v>
+      </c>
+      <c r="AB169">
+        <v>2</v>
+      </c>
+      <c r="AC169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:29">
       <c r="A170">
         <v>2024</v>
       </c>
@@ -11166,60 +11448,84 @@
       <c r="C170" t="s">
         <v>44</v>
       </c>
+      <c r="D170" t="s">
+        <v>31</v>
+      </c>
       <c r="E170" s="1">
-        <v>45528</v>
-      </c>
-      <c r="G170" s="3"/>
-      <c r="H170" s="3"/>
+        <v>45522</v>
+      </c>
+      <c r="F170" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="G170">
+        <v>26</v>
+      </c>
+      <c r="H170">
+        <v>2</v>
+      </c>
       <c r="I170">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="J170" t="s">
+        <v>44</v>
+      </c>
+      <c r="L170">
+        <v>46931</v>
       </c>
       <c r="S170" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="T170" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="171" spans="1:23">
+        <v>55</v>
+      </c>
+      <c r="U170" t="s">
+        <v>40</v>
+      </c>
+      <c r="V170" t="s">
+        <v>33</v>
+      </c>
+      <c r="X170" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y170">
+        <v>7</v>
+      </c>
+      <c r="Z170">
+        <v>1</v>
+      </c>
+      <c r="AA170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:29">
       <c r="A171">
         <v>2024</v>
       </c>
       <c r="B171" t="s">
-        <v>43</v>
-      </c>
-      <c r="C171" t="s">
-        <v>44</v>
-      </c>
-      <c r="D171" t="s">
-        <v>31</v>
+        <v>120</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E171" s="1">
-        <v>45535</v>
-      </c>
-      <c r="H171">
-        <v>3</v>
-      </c>
+        <v>45525</v>
+      </c>
+      <c r="G171" s="3"/>
+      <c r="H171" s="3"/>
       <c r="I171">
-        <v>25</v>
-      </c>
-      <c r="J171" t="s">
-        <v>44</v>
-      </c>
-      <c r="L171">
-        <v>46931</v>
+        <v>2</v>
       </c>
       <c r="S171" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="T171" t="s">
-        <v>57</v>
-      </c>
-      <c r="U171" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="172" spans="1:23">
+        <v>35</v>
+      </c>
+      <c r="W171" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="172" spans="1:29">
       <c r="A172">
         <v>2024</v>
       </c>
@@ -11229,35 +11535,22 @@
       <c r="C172" t="s">
         <v>44</v>
       </c>
-      <c r="D172" t="s">
-        <v>31</v>
-      </c>
       <c r="E172" s="1">
-        <v>45549</v>
-      </c>
-      <c r="H172">
-        <v>1</v>
-      </c>
+        <v>45528</v>
+      </c>
+      <c r="G172" s="3"/>
+      <c r="H172" s="3"/>
       <c r="I172">
-        <v>26</v>
-      </c>
-      <c r="J172" t="s">
-        <v>44</v>
-      </c>
-      <c r="L172">
-        <v>46931</v>
+        <v>24</v>
       </c>
       <c r="S172" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="T172" t="s">
-        <v>45</v>
-      </c>
-      <c r="U172" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="173" spans="1:23" hidden="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="173" spans="1:29">
       <c r="A173">
         <v>2024</v>
       </c>
@@ -11267,22 +11560,35 @@
       <c r="C173" t="s">
         <v>44</v>
       </c>
+      <c r="D173" t="s">
+        <v>31</v>
+      </c>
       <c r="E173" s="1">
-        <v>45556</v>
-      </c>
-      <c r="G173" s="3"/>
-      <c r="H173" s="3"/>
+        <v>45535</v>
+      </c>
+      <c r="H173">
+        <v>3</v>
+      </c>
       <c r="I173">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="J173" t="s">
+        <v>44</v>
+      </c>
+      <c r="L173">
+        <v>46931</v>
       </c>
       <c r="S173" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="T173" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="174" spans="1:23">
+        <v>57</v>
+      </c>
+      <c r="U173" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="174" spans="1:29">
       <c r="A174">
         <v>2024</v>
       </c>
@@ -11296,13 +11602,13 @@
         <v>31</v>
       </c>
       <c r="E174" s="1">
-        <v>45563</v>
+        <v>45549</v>
       </c>
       <c r="H174">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I174">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J174" t="s">
         <v>44</v>
@@ -11314,13 +11620,13 @@
         <v>35</v>
       </c>
       <c r="T174" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="U174" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="175" spans="1:23" hidden="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="175" spans="1:29">
       <c r="A175">
         <v>2024</v>
       </c>
@@ -11331,21 +11637,21 @@
         <v>44</v>
       </c>
       <c r="E175" s="1">
-        <v>45569</v>
+        <v>45556</v>
       </c>
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
       <c r="I175">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S175" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="T175" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="176" spans="1:23">
+    <row r="176" spans="1:29">
       <c r="A176">
         <v>2024</v>
       </c>
@@ -11359,13 +11665,13 @@
         <v>31</v>
       </c>
       <c r="E176" s="1">
-        <v>45584</v>
+        <v>45563</v>
       </c>
       <c r="H176">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I176">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J176" t="s">
         <v>44</v>
@@ -11377,13 +11683,13 @@
         <v>35</v>
       </c>
       <c r="T176" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="U176" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="177" spans="1:22" hidden="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="177" spans="1:22">
       <c r="A177">
         <v>2024</v>
       </c>
@@ -11394,15 +11700,15 @@
         <v>44</v>
       </c>
       <c r="E177" s="1">
-        <v>45590</v>
+        <v>45569</v>
       </c>
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
       <c r="I177">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="S177" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="T177" t="s">
         <v>35</v>
@@ -11422,13 +11728,13 @@
         <v>31</v>
       </c>
       <c r="E178" s="1">
-        <v>45602</v>
+        <v>45584</v>
       </c>
       <c r="H178">
         <v>1</v>
       </c>
       <c r="I178">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J178" t="s">
         <v>44</v>
@@ -11440,13 +11746,10 @@
         <v>35</v>
       </c>
       <c r="T178" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="U178" t="s">
-        <v>40</v>
-      </c>
-      <c r="V178" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="179" spans="1:22">
@@ -11459,35 +11762,22 @@
       <c r="C179" t="s">
         <v>44</v>
       </c>
-      <c r="D179" t="s">
+      <c r="E179" s="1">
+        <v>45590</v>
+      </c>
+      <c r="G179" s="3"/>
+      <c r="H179" s="3"/>
+      <c r="I179">
         <v>31</v>
       </c>
-      <c r="E179" s="1">
-        <v>45609</v>
-      </c>
-      <c r="H179">
-        <v>2</v>
-      </c>
-      <c r="I179">
-        <v>33</v>
-      </c>
-      <c r="J179" t="s">
-        <v>44</v>
-      </c>
-      <c r="L179">
-        <v>46931</v>
-      </c>
       <c r="S179" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="T179" t="s">
-        <v>70</v>
-      </c>
-      <c r="U179" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="180" spans="1:22" hidden="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="180" spans="1:22">
       <c r="A180">
         <v>2024</v>
       </c>
@@ -11497,19 +11787,35 @@
       <c r="C180" t="s">
         <v>44</v>
       </c>
+      <c r="D180" t="s">
+        <v>31</v>
+      </c>
       <c r="E180" s="1">
-        <v>45616</v>
-      </c>
-      <c r="G180" s="3"/>
-      <c r="H180" s="3"/>
+        <v>45602</v>
+      </c>
+      <c r="H180">
+        <v>1</v>
+      </c>
       <c r="I180">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="J180" t="s">
+        <v>44</v>
+      </c>
+      <c r="L180">
+        <v>46931</v>
       </c>
       <c r="S180" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="T180" t="s">
-        <v>35</v>
+        <v>83</v>
+      </c>
+      <c r="U180" t="s">
+        <v>40</v>
+      </c>
+      <c r="V180" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="181" spans="1:22">
@@ -11526,13 +11832,13 @@
         <v>31</v>
       </c>
       <c r="E181" s="1">
-        <v>45619</v>
+        <v>45609</v>
       </c>
       <c r="H181">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I181">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J181" t="s">
         <v>44</v>
@@ -11544,13 +11850,13 @@
         <v>35</v>
       </c>
       <c r="T181" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="U181" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="182" spans="1:22" hidden="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="182" spans="1:22">
       <c r="A182">
         <v>2024</v>
       </c>
@@ -11561,21 +11867,21 @@
         <v>44</v>
       </c>
       <c r="E182" s="1">
-        <v>45626</v>
+        <v>45616</v>
       </c>
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
       <c r="I182">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S182" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="T182" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="183" spans="1:22" hidden="1">
+    <row r="183" spans="1:22">
       <c r="A183">
         <v>2024</v>
       </c>
@@ -11585,19 +11891,32 @@
       <c r="C183" t="s">
         <v>44</v>
       </c>
+      <c r="D183" t="s">
+        <v>31</v>
+      </c>
       <c r="E183" s="1">
-        <v>45630</v>
-      </c>
-      <c r="G183" s="3"/>
-      <c r="H183" s="3"/>
+        <v>45619</v>
+      </c>
+      <c r="H183">
+        <v>3</v>
+      </c>
       <c r="I183">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="J183" t="s">
+        <v>44</v>
+      </c>
+      <c r="L183">
+        <v>46931</v>
       </c>
       <c r="S183" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="T183" t="s">
-        <v>35</v>
+        <v>128</v>
+      </c>
+      <c r="U183" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="184" spans="1:22">
@@ -11610,51 +11929,96 @@
       <c r="C184" t="s">
         <v>44</v>
       </c>
-      <c r="D184" t="s">
-        <v>31</v>
-      </c>
       <c r="E184" s="1">
-        <v>45634</v>
-      </c>
-      <c r="H184">
-        <v>1</v>
-      </c>
+        <v>45626</v>
+      </c>
+      <c r="G184" s="3"/>
+      <c r="H184" s="3"/>
       <c r="I184">
-        <v>38</v>
-      </c>
-      <c r="J184" t="s">
-        <v>44</v>
-      </c>
-      <c r="L184">
-        <v>46931</v>
+        <v>36</v>
       </c>
       <c r="S184" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="T184" t="s">
-        <v>66</v>
-      </c>
-      <c r="U184" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="185" spans="1:22" hidden="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="185" spans="1:22">
+      <c r="A185">
+        <v>2024</v>
+      </c>
+      <c r="B185" t="s">
+        <v>43</v>
+      </c>
+      <c r="C185" t="s">
+        <v>44</v>
+      </c>
+      <c r="E185" s="1">
+        <v>45630</v>
+      </c>
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
+      <c r="I185">
+        <v>37</v>
+      </c>
+      <c r="S185" t="s">
+        <v>67</v>
+      </c>
+      <c r="T185" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="186" spans="1:22">
+      <c r="A186">
+        <v>2024</v>
+      </c>
+      <c r="B186" t="s">
+        <v>43</v>
+      </c>
+      <c r="C186" t="s">
+        <v>44</v>
+      </c>
+      <c r="D186" t="s">
+        <v>31</v>
+      </c>
+      <c r="E186" s="1">
+        <v>45634</v>
+      </c>
+      <c r="H186">
+        <v>1</v>
+      </c>
+      <c r="I186">
+        <v>38</v>
+      </c>
+      <c r="J186" t="s">
+        <v>44</v>
+      </c>
+      <c r="L186">
+        <v>46931</v>
+      </c>
+      <c r="S186" t="s">
+        <v>35</v>
+      </c>
+      <c r="T186" t="s">
+        <v>66</v>
+      </c>
+      <c r="U186" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="187" spans="1:22">
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC185" xr:uid="{301F969D-DFCA-4A79-8310-530A765857C0}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Nilton Santos"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC185">
-      <sortCondition ref="E1:E185"/>
+  <autoFilter ref="A1:AC187" xr:uid="{301F969D-DFCA-4A79-8310-530A765857C0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC187">
+      <sortCondition ref="E1:E187"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC185">
-    <sortCondition ref="E1:E185"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC187">
+    <sortCondition ref="E1:E187"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>